<commit_message>
Made a better downtrend prediction model
</commit_message>
<xml_diff>
--- a/Supplemental/btc_correction_dates.xlsx
+++ b/Supplemental/btc_correction_dates.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Isaac/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Isaac/Desktop/Crypto_Analysis-master/Supplemental/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{415E223F-6A2F-C04B-AC29-B9FF216E92B3}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{C4760541-F54A-8043-9852-FCB6C6FCA25A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5480" yWindow="460" windowWidth="25380" windowHeight="16580" xr2:uid="{B4CC3477-DB8E-7B45-87A3-C4E621D3AC69}"/>
+    <workbookView xWindow="19740" yWindow="460" windowWidth="10000" windowHeight="17040" xr2:uid="{7952EF89-2D49-AB45-BDB0-66CF20D30E15}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -45,28 +45,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -96,12 +81,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,272 +398,389 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F627D57E-DEB0-B544-881D-F84A8A7F5FDA}">
-  <dimension ref="A1:B32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF5D4757-6840-B04D-8E47-09D32F82EB59}">
+  <dimension ref="A1:B47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="149" zoomScaleNormal="149" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="2" width="10.83203125" style="4"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="3">
+      <c r="A2" s="1">
+        <v>40489</v>
+      </c>
+      <c r="B2" s="1">
+        <v>40492</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>40510</v>
+      </c>
+      <c r="B3" s="1">
+        <v>40522</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>40559</v>
+      </c>
+      <c r="B4" s="1">
+        <v>40562</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>40591</v>
+      </c>
+      <c r="B5" s="1">
+        <v>40595</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>40599</v>
+      </c>
+      <c r="B6" s="1">
+        <v>40623</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>40627</v>
+      </c>
+      <c r="B7" s="1">
+        <v>40638</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>40677</v>
+      </c>
+      <c r="B8" s="1">
+        <v>40684</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>40703</v>
+      </c>
+      <c r="B9" s="1">
+        <v>40706</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>40707</v>
+      </c>
+      <c r="B10" s="1">
+        <v>40762</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>40775</v>
+      </c>
+      <c r="B11" s="1">
+        <v>40865</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>40916</v>
+      </c>
+      <c r="B12" s="1">
+        <v>40957</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>40982</v>
+      </c>
+      <c r="B13" s="1">
+        <v>40993</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>41138</v>
+      </c>
+      <c r="B14" s="1">
+        <v>41140</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>41186</v>
+      </c>
+      <c r="B15" s="1">
+        <v>41208</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="2">
         <v>41373</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B16" s="2">
         <v>41380</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
         <v>41388</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B17" s="2">
         <v>41397</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
         <v>41420</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B18" s="2">
         <v>41461</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
         <v>41517</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B19" s="2">
         <v>41549</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
         <v>41596</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B20" s="2">
         <v>41597</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
         <v>41612</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B21" s="2">
         <v>41615</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
         <v>41618</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B22" s="2">
         <v>41626</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
         <v>41645</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B23" s="2">
         <v>41694</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
         <v>41701</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B24" s="2">
         <v>41739</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
         <v>41745</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B25" s="2">
         <v>41778</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="2">
         <v>41793</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B26" s="2">
         <v>41815</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="2">
         <v>41822</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B27" s="2">
         <v>41917</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
         <v>41926</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B28" s="2">
         <v>41945</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="2">
         <v>41955</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B29" s="2">
         <v>42018</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="2">
         <v>42030</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B30" s="2">
         <v>42035</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="2">
         <v>42074</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B31" s="2">
         <v>42156</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="2">
         <v>42197</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B32" s="2">
         <v>42234</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="2">
         <v>42312</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B33" s="2">
         <v>42332</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" s="3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="2">
         <v>42353</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B34" s="2">
         <v>42364</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" s="3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="2">
         <v>42376</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B35" s="2">
         <v>42384</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="2">
         <v>42389</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B36" s="2">
         <v>42400</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="2">
         <v>42422</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B37" s="2">
         <v>42434</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="2">
         <v>42538</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B38" s="2">
         <v>42543</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="2">
         <v>42553</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B39" s="2">
         <v>42614</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="2">
         <v>42739</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B40" s="2">
         <v>42746</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="2">
         <v>42797</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B41" s="2">
         <v>42818</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="2">
         <v>42897</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B42" s="2">
         <v>42932</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="2">
         <v>42979</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B43" s="2">
         <v>42992</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A30" s="3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="2">
         <v>43047</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B44" s="2">
         <v>43051</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A31" s="3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="2">
         <v>43085</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B45" s="2">
         <v>43099</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="2">
         <v>43106</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B46" s="2">
         <v>43136</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="2">
+        <v>43163</v>
+      </c>
+      <c r="B47" s="2">
+        <v>43196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>